<commit_message>
Actualización de template y agregado de nuevos templates
</commit_message>
<xml_diff>
--- a/templates/template_import_data_dry.xlsx
+++ b/templates/template_import_data_dry.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DescargasNavegador\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesus\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0406DA18-B8D7-4E2E-8629-F4BFD84B1B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Secados" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Único</t>
   </si>
@@ -48,13 +49,19 @@
   </si>
   <si>
     <t>Práctico</t>
+  </si>
+  <si>
+    <t>Altura de la Madre</t>
+  </si>
+  <si>
+    <t>Condición de la Madre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +80,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,16 +121,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -128,16 +147,16 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -173,17 +192,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Animales" displayName="Animales" ref="A1:H11" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:H11"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="Único" dataDxfId="7"/>
-    <tableColumn id="5" name="ID Electrónico" dataDxfId="0"/>
-    <tableColumn id="4" name="Práctico" dataDxfId="1"/>
-    <tableColumn id="2" name="Fecha" dataDxfId="6"/>
-    <tableColumn id="3" name="Peso de la Madre" dataDxfId="5"/>
-    <tableColumn id="8" name="Técnico" dataDxfId="4"/>
-    <tableColumn id="9" name="Comentario" dataDxfId="3"/>
-    <tableColumn id="10" name="Lote" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Animales" displayName="Animales" ref="A1:J11" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A1:J11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Único" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ID Electrónico" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Práctico" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Fecha" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Peso de la Madre" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{F2A4CD4B-5AF8-420A-A66F-A427259DA2B8}" name="Altura de la Madre" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{A7A1FFF8-F467-4D67-AAB6-626AC600D23E}" name="Condición de la Madre" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Técnico" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Comentario" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Lote" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -451,150 +472,176 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6"/>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6"/>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
       <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -602,8 +649,11 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>